<commit_message>
Docs from the FCPS website
</commit_message>
<xml_diff>
--- a/doc/Links.xlsx
+++ b/doc/Links.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>http://www.ddschools.org/district/referendum/property_values</t>
   </si>
@@ -54,6 +54,18 @@
   </si>
   <si>
     <t>Post article listing immersion schools by county</t>
+  </si>
+  <si>
+    <t>Site Design</t>
+  </si>
+  <si>
+    <t>http://data.baltimoresun.com/ga-session-issues-2015/</t>
+  </si>
+  <si>
+    <t>From http://damihere.com/</t>
+  </si>
+  <si>
+    <t>http://interactives.dallasnews.com/2015/topletz-homes/</t>
   </si>
 </sst>
 </file>
@@ -371,16 +383,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="127.5703125" customWidth="1"/>
-    <col min="2" max="2" width="60" customWidth="1"/>
+    <col min="2" max="2" width="93.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -423,6 +435,24 @@
         <v>9</v>
       </c>
     </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>